<commit_message>
added new version for part 4 of 460
</commit_message>
<xml_diff>
--- a/460/Week_1/Assignment_1_Diet.xlsx
+++ b/460/Week_1/Assignment_1_Diet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyoung\Desktop\school\Northwestern\MSDS_460\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyoung\Desktop\school\Northwestern\Northwestern_MSDS\460\Week_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45CDFDC-F5E0-4EE1-8D68-5B0ACB60820D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028AF7D1-7F16-4D8E-8093-B0B912764F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="3030" windowWidth="23520" windowHeight="12645" xr2:uid="{48179C16-4BB1-4FBA-89E1-6B994EE11169}"/>
+    <workbookView xWindow="2925" yWindow="3375" windowWidth="23520" windowHeight="12645" xr2:uid="{48179C16-4BB1-4FBA-89E1-6B994EE11169}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,12 +375,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -397,31 +391,37 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D3E280-5622-4EFE-AF65-3A9D48717B7E}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,33 +785,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="14" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="4" t="s">
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
@@ -822,62 +822,62 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="17"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="8">
         <v>1.33</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="13" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="14">
         <v>2.25</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="15">
         <v>3.5</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Q3" s="6">
         <v>0.2</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -885,55 +885,55 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>170</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>1360</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>70</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="7">
         <v>210</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="10">
         <v>196</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="10">
         <v>784</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="12">
         <v>540</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="P4" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>0</v>
-      </c>
-      <c r="R4" s="7">
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
         <v>0</v>
       </c>
     </row>
@@ -941,55 +941,55 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>100</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>100</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>800</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>800</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>70</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>70</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="7">
         <v>210</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>210</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="10">
         <v>122</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="10">
         <v>122</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="10">
         <v>488</v>
       </c>
-      <c r="M5" s="16">
-        <v>0</v>
-      </c>
-      <c r="N5" s="16">
-        <v>0</v>
-      </c>
-      <c r="O5" s="16">
-        <v>0</v>
-      </c>
-      <c r="P5" s="7">
+      <c r="M5" s="12">
+        <v>0</v>
+      </c>
+      <c r="N5" s="12">
+        <v>0</v>
+      </c>
+      <c r="O5" s="12">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5">
         <v>170</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="5">
         <v>170</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="5">
         <v>3400</v>
       </c>
     </row>
@@ -997,55 +997,55 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>7000</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>56000</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>4000</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>12000</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="10">
         <v>23000</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="M6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="16">
+      <c r="N6" s="12">
         <v>12000</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="O6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="P6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="5">
         <v>6000</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="R6" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1053,55 +1053,55 @@
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>0.1</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>0.8</v>
       </c>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-      <c r="G7" s="9">
-        <v>0</v>
-      </c>
-      <c r="H7" s="9">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
-        <v>0</v>
-      </c>
-      <c r="J7" s="13" t="s">
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="10">
         <v>0.1</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="12">
         <v>18.399999999999999</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="12">
         <v>73.599999999999994</v>
       </c>
-      <c r="P7" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="7">
-        <v>0</v>
-      </c>
-      <c r="R7" s="7">
+      <c r="P7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0</v>
+      </c>
+      <c r="R7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1109,55 +1109,55 @@
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>200</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>1600</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>130</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="7">
         <v>390</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="10">
         <v>6</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="16">
-        <v>0</v>
-      </c>
-      <c r="N8" s="16">
-        <v>0</v>
-      </c>
-      <c r="O8" s="16">
-        <v>0</v>
-      </c>
-      <c r="P8" s="7" t="s">
+      <c r="M8" s="12">
+        <v>0</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="5">
         <v>20</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="R8" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1165,55 +1165,55 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>0.1</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>0.8</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>0.9</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>2.7</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="10">
         <v>0.4</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="12">
         <v>0.1</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="O9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="P9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="5">
         <v>1.7</v>
       </c>
-      <c r="R9" s="7" t="s">
+      <c r="R9" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1221,55 +1221,55 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>30</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>2000</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="7">
         <v>260</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="7">
         <v>780</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="10">
         <v>376</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="10">
         <v>1504</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="12">
         <v>190</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="O10" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="P10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="5">
         <v>170</v>
       </c>
-      <c r="R10" s="7" t="s">
+      <c r="R10" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1277,7 +1277,7 @@
       <c r="B12" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>3</v>
       </c>
       <c r="D12" t="s">
@@ -1289,13 +1289,13 @@
       <c r="F12" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="9">
         <v>5</v>
       </c>
       <c r="H12" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="11">
         <v>2</v>
       </c>
       <c r="J12" t="s">
@@ -1304,7 +1304,7 @@
       <c r="K12" s="3">
         <v>6</v>
       </c>
-      <c r="L12" s="20" t="s">
+      <c r="L12" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
       <c r="A21" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1621,7 +1621,7 @@
       <c r="A24" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>39</v>
       </c>
       <c r="I24" t="s">
@@ -1635,7 +1635,7 @@
       <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I25" t="s">

</xml_diff>